<commit_message>
Latest code 28Nov 2024
</commit_message>
<xml_diff>
--- a/AutomationDemo/TestData/TestInfo.xlsx
+++ b/AutomationDemo/TestData/TestInfo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\AutomationDemo\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sudha Arya\git\repository\AutomationDemo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99485EED-C350-407F-ACDF-30B4C684CBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FECED22-2767-4A5A-9142-8FC9AB62CA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Demo12</t>
-  </si>
-  <si>
-    <t>Demo1234</t>
   </si>
   <si>
     <t>Test123456$</t>
@@ -360,7 +357,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,15 +379,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -398,7 +395,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>